<commit_message>
CSS Update, Gut Old & Update Bootstrap
</commit_message>
<xml_diff>
--- a/TimeTracking.xlsx
+++ b/TimeTracking.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Time</t>
   </si>
@@ -95,13 +95,19 @@
     <t>Didn't need at all, only needed the Load method for datatable - code commented (OrderSearches)</t>
   </si>
   <si>
-    <t>Create Pages &amp; Display Data</t>
-  </si>
-  <si>
-    <t>Change Bootstrap</t>
-  </si>
-  <si>
     <t>Angular &amp; WebAPI Firing Together</t>
+  </si>
+  <si>
+    <t>Create Pages &amp; Gut Old App Stuff</t>
+  </si>
+  <si>
+    <t>https://www.cssmatic.com/noise-texture</t>
+  </si>
+  <si>
+    <t>Change Bootstrap &amp; Custom CSS</t>
+  </si>
+  <si>
+    <t>Finish Pages And Display Data Nicely</t>
   </si>
 </sst>
 </file>
@@ -459,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +632,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -637,7 +643,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
@@ -646,13 +652,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>